<commit_message>
setting up for file cleaning
</commit_message>
<xml_diff>
--- a/Kid Choice Experiments/quick kid graphs.xlsx
+++ b/Kid Choice Experiments/quick kid graphs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
   <si>
     <t>&gt; table(maintable$Condition, maintable$choseObjectDrop)</t>
   </si>
@@ -109,6 +109,15 @@
   </si>
   <si>
     <t>Does correctness differ by age? Doesn't seem like, still collecting data</t>
+  </si>
+  <si>
+    <t>Object Ambiguous</t>
+  </si>
+  <si>
+    <t>Subject Ambiguous</t>
+  </si>
+  <si>
+    <t>CONTROL EXP</t>
   </si>
 </sst>
 </file>
@@ -221,10 +230,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>OD</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>SD</c:v>
+                  <c:v>Subject Ambiguous</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Object Ambiguous</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -266,10 +275,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>OD</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>SD</c:v>
+                  <c:v>Subject Ambiguous</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Object Ambiguous</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -311,10 +320,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>OD</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>SD</c:v>
+                  <c:v>Subject Ambiguous</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Object Ambiguous</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -344,11 +353,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2122486968"/>
-        <c:axId val="2122486536"/>
+        <c:axId val="2117514616"/>
+        <c:axId val="2117517640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2122486968"/>
+        <c:axId val="2117514616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -357,7 +366,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2122486536"/>
+        <c:crossAx val="2117517640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -365,7 +374,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2122486536"/>
+        <c:axId val="2117517640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -376,7 +385,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2122486968"/>
+        <c:crossAx val="2117514616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -599,11 +608,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2116807688"/>
-        <c:axId val="2116963032"/>
+        <c:axId val="2115801592"/>
+        <c:axId val="2115804568"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2116807688"/>
+        <c:axId val="2115801592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -612,7 +621,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2116963032"/>
+        <c:crossAx val="2115804568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -620,7 +629,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2116963032"/>
+        <c:axId val="2115804568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -631,7 +640,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2116807688"/>
+        <c:crossAx val="2115801592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -818,11 +827,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2113013432"/>
-        <c:axId val="-2113732664"/>
+        <c:axId val="2115847448"/>
+        <c:axId val="2115850424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2113013432"/>
+        <c:axId val="2115847448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -831,7 +840,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2113732664"/>
+        <c:crossAx val="2115850424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -839,7 +848,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2113732664"/>
+        <c:axId val="2115850424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -850,7 +859,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2113013432"/>
+        <c:crossAx val="2115847448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1037,11 +1046,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2119830024"/>
-        <c:axId val="2120135128"/>
+        <c:axId val="2115881656"/>
+        <c:axId val="2117558136"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2119830024"/>
+        <c:axId val="2115881656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1050,7 +1059,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2120135128"/>
+        <c:crossAx val="2117558136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1058,7 +1067,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2120135128"/>
+        <c:axId val="2117558136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1069,7 +1078,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2119830024"/>
+        <c:crossAx val="2115881656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1185,16 +1194,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>812800</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1540,8 +1549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D11" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
+      <selection activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1570,7 +1579,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H3">
         <v>16</v>
@@ -1587,7 +1596,7 @@
         <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="H4">
         <v>21</v>
@@ -1704,6 +1713,9 @@
     <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>11</v>
+      </c>
+      <c r="G14" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:10">

</xml_diff>

<commit_message>
updating analyses w/ kids thru 10/20ish
</commit_message>
<xml_diff>
--- a/Kid Choice Experiments/quick kid graphs.xlsx
+++ b/Kid Choice Experiments/quick kid graphs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="8280" yWindow="420" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -245,10 +245,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>21.0</c:v>
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -293,7 +293,7 @@
                   <c:v>15.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.0</c:v>
+                  <c:v>19.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -338,7 +338,7 @@
                   <c:v>19.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.0</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -353,11 +353,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2117514616"/>
-        <c:axId val="2117517640"/>
+        <c:axId val="2115532744"/>
+        <c:axId val="2121238216"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2117514616"/>
+        <c:axId val="2115532744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -366,7 +366,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117517640"/>
+        <c:crossAx val="2121238216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -374,7 +374,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2117517640"/>
+        <c:axId val="2121238216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -385,7 +385,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117514616"/>
+        <c:crossAx val="2115532744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -473,13 +473,13 @@
                   <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.0</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.0</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -530,7 +530,7 @@
                   <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>8.0</c:v>
@@ -584,10 +584,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>9.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11.0</c:v>
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>15.0</c:v>
@@ -608,11 +608,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2115801592"/>
-        <c:axId val="2115804568"/>
+        <c:axId val="2080996744"/>
+        <c:axId val="2080999720"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2115801592"/>
+        <c:axId val="2080996744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -621,7 +621,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115804568"/>
+        <c:crossAx val="2080999720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -629,7 +629,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2115804568"/>
+        <c:axId val="2080999720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -640,7 +640,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115801592"/>
+        <c:crossAx val="2080996744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -719,10 +719,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.0</c:v>
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -764,7 +764,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>5.0</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>6.0</c:v>
@@ -809,10 +809,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>9.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11.0</c:v>
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -827,11 +827,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2115847448"/>
-        <c:axId val="2115850424"/>
+        <c:axId val="2080971256"/>
+        <c:axId val="2120318760"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2115847448"/>
+        <c:axId val="2080971256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -840,7 +840,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115850424"/>
+        <c:crossAx val="2120318760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -848,7 +848,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2115850424"/>
+        <c:axId val="2120318760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -859,7 +859,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115847448"/>
+        <c:crossAx val="2080971256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -938,7 +938,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>4.0</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2.0</c:v>
@@ -983,7 +983,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>6.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>5.0</c:v>
@@ -1028,10 +1028,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>9.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
                   <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1046,11 +1046,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2115881656"/>
-        <c:axId val="2117558136"/>
+        <c:axId val="2122287000"/>
+        <c:axId val="2121363848"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2115881656"/>
+        <c:axId val="2122287000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1059,7 +1059,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117558136"/>
+        <c:crossAx val="2121363848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1067,7 +1067,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2117558136"/>
+        <c:axId val="2121363848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1078,7 +1078,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115881656"/>
+        <c:crossAx val="2122287000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1549,8 +1549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
-      <selection activeCell="K44" sqref="K44"/>
+    <sheetView tabSelected="1" topLeftCell="E13" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1582,7 +1582,7 @@
         <v>31</v>
       </c>
       <c r="H3">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I3">
         <v>15</v>
@@ -1599,13 +1599,13 @@
         <v>30</v>
       </c>
       <c r="H4">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="I4">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J4">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -1656,7 +1656,7 @@
         <v>6</v>
       </c>
       <c r="J10">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1667,13 +1667,13 @@
         <v>27</v>
       </c>
       <c r="H11">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I11">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J11">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1684,7 +1684,7 @@
         <v>25</v>
       </c>
       <c r="H12">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I12">
         <v>8</v>
@@ -1701,7 +1701,7 @@
         <v>24</v>
       </c>
       <c r="H13">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I13">
         <v>12</v>
@@ -1745,13 +1745,13 @@
         <v>18</v>
       </c>
       <c r="H17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I17">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J17">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1762,13 +1762,13 @@
         <v>19</v>
       </c>
       <c r="H18">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I18">
         <v>6</v>
       </c>
       <c r="J18">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1803,13 +1803,13 @@
         <v>24</v>
       </c>
       <c r="H22">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I22">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J22">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1826,7 +1826,7 @@
         <v>5</v>
       </c>
       <c r="J23">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>